<commit_message>
Add CO municipality-level data
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E78F7C-ABC0-43C2-9AF1-2DEB438B4113}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87ACAE9-4060-41CD-992D-D148383992F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J65" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J65" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J66" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:J65"/>
+      <selection activeCell="A66" sqref="A66:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,6 +2797,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>43966</v>
+      </c>
+      <c r="B66" s="12">
+        <v>68852</v>
+      </c>
+      <c r="C66" s="13">
+        <v>1151</v>
+      </c>
+      <c r="D66" s="13">
+        <v>1465</v>
+      </c>
+      <c r="E66" s="13">
+        <v>0</v>
+      </c>
+      <c r="F66" s="13">
+        <v>27</v>
+      </c>
+      <c r="G66" s="13">
+        <v>6</v>
+      </c>
+      <c r="H66" s="13">
+        <v>2</v>
+      </c>
+      <c r="I66" s="13">
+        <v>103</v>
+      </c>
+      <c r="J66" s="13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update data, docs and metadata->index
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87ACAE9-4060-41CD-992D-D148383992F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E4D7BB-A0BD-427C-8791-9483B4B0D627}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J66" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J68" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:J66"/>
+      <selection activeCell="A68" sqref="A68:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,6 +2829,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>43967</v>
+      </c>
+      <c r="B67" s="15">
+        <v>69363</v>
+      </c>
+      <c r="C67" s="16">
+        <v>511</v>
+      </c>
+      <c r="D67" s="16">
+        <v>1466</v>
+      </c>
+      <c r="E67" s="16">
+        <v>1</v>
+      </c>
+      <c r="F67" s="16">
+        <v>26</v>
+      </c>
+      <c r="G67" s="16">
+        <v>5</v>
+      </c>
+      <c r="H67" s="16">
+        <v>1</v>
+      </c>
+      <c r="I67" s="16">
+        <v>104</v>
+      </c>
+      <c r="J67" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="11">
+        <v>43968</v>
+      </c>
+      <c r="B68" s="12">
+        <v>69842</v>
+      </c>
+      <c r="C68" s="13">
+        <v>479</v>
+      </c>
+      <c r="D68" s="13">
+        <v>1466</v>
+      </c>
+      <c r="E68" s="13">
+        <v>0</v>
+      </c>
+      <c r="F68" s="13">
+        <v>25</v>
+      </c>
+      <c r="G68" s="13">
+        <v>5</v>
+      </c>
+      <c r="H68" s="13">
+        <v>1</v>
+      </c>
+      <c r="I68" s="13">
+        <v>104</v>
+      </c>
+      <c r="J68" s="13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update data and enable cache of daily sources
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E4D7BB-A0BD-427C-8791-9483B4B0D627}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1680379-6717-4649-AB5E-934A41657532}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J68" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J68" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J69" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J69" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:J68"/>
+      <selection activeCell="A69" sqref="A69:J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,6 +2893,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <v>43969</v>
+      </c>
+      <c r="B69" s="15">
+        <v>70970</v>
+      </c>
+      <c r="C69" s="16">
+        <v>1128</v>
+      </c>
+      <c r="D69" s="16">
+        <v>1467</v>
+      </c>
+      <c r="E69" s="16">
+        <v>1</v>
+      </c>
+      <c r="F69" s="16">
+        <v>24</v>
+      </c>
+      <c r="G69" s="16">
+        <v>5</v>
+      </c>
+      <c r="H69" s="16">
+        <v>1</v>
+      </c>
+      <c r="I69" s="16">
+        <v>104</v>
+      </c>
+      <c r="J69" s="16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add backcompat and data subsets
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D34469-DC31-4E29-931A-E3B9405CA914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +85,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -186,6 +191,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -201,8 +215,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -217,8 +229,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -233,8 +243,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -249,8 +257,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -265,8 +271,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -281,8 +285,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -297,8 +299,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -313,8 +313,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -329,8 +327,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -345,8 +341,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
@@ -363,8 +357,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -379,8 +371,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -399,8 +389,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J70" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J70" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J71">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +403,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+      <selection activeCell="A71" sqref="A71:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +2947,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <v>43971</v>
+      </c>
+      <c r="B71" s="21">
+        <v>72860</v>
+      </c>
+      <c r="C71" s="22">
+        <v>909</v>
+      </c>
+      <c r="D71" s="22">
+        <v>1468</v>
+      </c>
+      <c r="E71" s="22">
+        <v>0</v>
+      </c>
+      <c r="F71" s="22">
+        <v>21</v>
+      </c>
+      <c r="G71" s="22">
+        <v>3</v>
+      </c>
+      <c r="H71" s="22">
+        <v>2</v>
+      </c>
+      <c r="I71" s="22">
+        <v>106</v>
+      </c>
+      <c r="J71" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalise update to V2
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D34469-DC31-4E29-931A-E3B9405CA914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -60,11 +59,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +85,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -186,6 +191,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
@@ -201,8 +215,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -217,8 +229,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -233,8 +243,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -249,8 +257,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -265,8 +271,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -281,8 +285,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -297,8 +299,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -313,8 +313,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -329,8 +327,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -345,8 +341,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
@@ -363,8 +357,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -379,8 +371,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri Light"/>
-        <family val="2"/>
-        <charset val="238"/>
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -399,8 +389,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J70" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J70" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J71">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,16 +403,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -695,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+      <selection activeCell="A71" sqref="A71:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +2947,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <v>43971</v>
+      </c>
+      <c r="B71" s="21">
+        <v>72860</v>
+      </c>
+      <c r="C71" s="22">
+        <v>909</v>
+      </c>
+      <c r="D71" s="22">
+        <v>1468</v>
+      </c>
+      <c r="E71" s="22">
+        <v>0</v>
+      </c>
+      <c r="F71" s="22">
+        <v>21</v>
+      </c>
+      <c r="G71" s="22">
+        <v>3</v>
+      </c>
+      <c r="H71" s="22">
+        <v>2</v>
+      </c>
+      <c r="I71" s="22">
+        <v>106</v>
+      </c>
+      <c r="J71" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor wikidata-based pipelines and update data
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F00C1F-3D2A-4E8A-85C9-D5CC975AEEA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -132,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -198,6 +199,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -389,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J72" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -403,16 +413,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -685,11 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:J71"/>
+      <selection activeCell="A72" sqref="A72:J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,6 +2989,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="23">
+        <v>43972</v>
+      </c>
+      <c r="B72" s="24">
+        <v>73742</v>
+      </c>
+      <c r="C72" s="25">
+        <v>882</v>
+      </c>
+      <c r="D72" s="25">
+        <v>1468</v>
+      </c>
+      <c r="E72" s="25">
+        <v>0</v>
+      </c>
+      <c r="F72" s="25">
+        <v>21</v>
+      </c>
+      <c r="G72" s="25">
+        <v>4</v>
+      </c>
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+      <c r="I72" s="25">
+        <v>106</v>
+      </c>
+      <c r="J72" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor wikidata-based pipelines and update data (#45)
* Refactor wikidata-based pipelines and update data

* Enable testing for pull requests

* Fix weather pipeline

* Update weather and speed up forecast

* Fix V1 mobility and disable master.json
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F00C1F-3D2A-4E8A-85C9-D5CC975AEEA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -132,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -198,6 +199,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -389,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J72" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -403,16 +413,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -685,11 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:J71"/>
+      <selection activeCell="A72" sqref="A72:J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,6 +2989,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="23">
+        <v>43972</v>
+      </c>
+      <c r="B72" s="24">
+        <v>73742</v>
+      </c>
+      <c r="C72" s="25">
+        <v>882</v>
+      </c>
+      <c r="D72" s="25">
+        <v>1468</v>
+      </c>
+      <c r="E72" s="25">
+        <v>0</v>
+      </c>
+      <c r="F72" s="25">
+        <v>21</v>
+      </c>
+      <c r="G72" s="25">
+        <v>4</v>
+      </c>
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+      <c r="I72" s="25">
+        <v>106</v>
+      </c>
+      <c r="J72" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sync development branch (#47)
* Add backcompat and data subsets

* Add hospitalization data

* Move hospitalization to its own branch

* Refactor wikidata-based pipelines and update data (#45)

* Refactor wikidata-based pipelines and update data

* Enable testing for pull requests

* Fix weather pipeline

* Update weather and speed up forecast

* Fix V1 mobility and disable master.json
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F00C1F-3D2A-4E8A-85C9-D5CC975AEEA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -132,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -198,6 +199,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -389,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J72" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -403,16 +413,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -685,11 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:J71"/>
+      <selection activeCell="A72" sqref="A72:J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,6 +2989,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="23">
+        <v>43972</v>
+      </c>
+      <c r="B72" s="24">
+        <v>73742</v>
+      </c>
+      <c r="C72" s="25">
+        <v>882</v>
+      </c>
+      <c r="D72" s="25">
+        <v>1468</v>
+      </c>
+      <c r="E72" s="25">
+        <v>0</v>
+      </c>
+      <c r="F72" s="25">
+        <v>21</v>
+      </c>
+      <c r="G72" s="25">
+        <v>4</v>
+      </c>
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+      <c r="I72" s="25">
+        <v>106</v>
+      </c>
+      <c r="J72" s="25">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatic data update (#51)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654FC9E3-1792-4C0A-8F62-962376F54392}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097731B8-C1EF-4A1D-872A-99C6B92E68A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J73" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J73" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J74" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J74" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J73" sqref="A73:J73"/>
+      <selection activeCell="A74" sqref="A74:J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3053,6 +3053,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="17">
+        <v>43974</v>
+      </c>
+      <c r="B74" s="18">
+        <v>74760</v>
+      </c>
+      <c r="C74" s="19">
+        <v>341</v>
+      </c>
+      <c r="D74" s="19">
+        <v>1468</v>
+      </c>
+      <c r="E74" s="19">
+        <v>0</v>
+      </c>
+      <c r="F74" s="19">
+        <v>18</v>
+      </c>
+      <c r="G74" s="19">
+        <v>4</v>
+      </c>
+      <c r="H74" s="19">
+        <v>0</v>
+      </c>
+      <c r="I74" s="19">
+        <v>107</v>
+      </c>
+      <c r="J74" s="19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>